<commit_message>
cds multi filter changes till now for 1-3
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC02_CDS_study-CIDR_LibraryStrategy-NotSpecifiedindata_Gender-Female_SampleTumor-Normal.xlsx
+++ b/InputFiles/CDS/TC02_CDS_study-CIDR_LibraryStrategy-NotSpecifiedindata_Gender-Female_SampleTumor-Normal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podagatlapalll2\CDS Automation\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\MarchBranch\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1E4385-7D5A-472E-9871-F4AA123F061F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A4F124-1DD6-4F02-87C9-8570DF0280F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
@@ -57,94 +57,483 @@
     <t>ParticipantsTab</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
+    <t>TC02_CDSPHSAccession2250_LibraryStrategy-NotSpecifiedindata_Gender-Female_SampleTumor-Normal_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC02_CDSPHSAccession2250_LibraryStrategy-NotSpecifiedindata_Gender-Female_SampleTumor-Normal_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>WITH {
+    phs_accession: "phs002250",
+    subject_ids: [],
+    experimental_strategies: [],
+    gender: ["Female"],
+    sample_tumor_status: ["Normal"],
+    file_types: [],
+    library_strategies: ["Not specified in data],
+    library_sources: [],
+    library_selections: [],
+    library_layouts: [],
+    platforms: [],
+    instrument_models: [],
+    reference_genome_assemblies: [],
+    primary_diagnoses: [],
+    num_study_samples_min: 0,
+    num_study_samples_max: 0,
+    num_study_participants_max: 0,
+    num_study_participants_min: 0
+} AS inputs, "Not specified in data" AS na
+MATCH (s:study {phs_accession: inputs.phs_accession})
+OPTIONAL MATCH (s)&lt;--(p:participant)
+WITH inputs, na, s, count(distinct p) AS num_p
+WHERE
+    (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+    (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH inputs, na, s, count(distinct samp) AS num_samp
+WHERE
+    (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+    (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH inputs, na, samp, {
+	sample_id: samp.sample_id,
+	study_name: s.study_name,
+	accession: s.phs_accession,
+	tumor: samp.sample_tumor_status,
+	analyte_type: samp.sample_type
+} AS data
+WHERE
+    (size(inputs.sample_tumor_status) = 0 OR samp.sample_tumor_status IN inputs.sample_tumor_status)
+OPTIONAL MATCH (samp)--&gt;(p:participant)
+WITH inputs, na, samp, 
+	apoc.map.merge(data, {
+		participant_id: p.participant_id
+	}) AS data,
+	COLLECT(DISTINCT p.participant_id) AS participant_id,
+	COLLECT(DISTINCT p.gender) AS gender
+WHERE 
+    (size(inputs.subject_ids) = 0 OR size(apoc.coll.intersection(inputs.participant_id, participant_id)) &gt; 0) AND
+    (size(inputs.gender) = 0 OR size(apoc.coll.intersection(inputs.gender, gender)) &gt; 0)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH inputs, na, samp, data,
+	COLLECT(DISTINCT f.file_type) AS file_types, 
+	apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+WHERE
+	(size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+    (size(inputs.file_types) = 0 OR size(apoc.coll.intersection(inputs.file_types, file_types)) &gt; 0)
+OPTIONAL MATCH (samp)&lt;--(:file)&lt;--(g:genomic_info)
+WITH inputs, na, samp, data,
+	COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+	COLLECT(DISTINCT g.library_source) AS library_source,
+	COLLECT(DISTINCT g.library_selection) AS library_selection,
+	COLLECT(DISTINCT g.library_layout) AS library_layout,
+	COLLECT(DISTINCT g.platform) AS platform,
+	COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+	COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+WHERE
+    (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+    (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND 
+    (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+    (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+    (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+    (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+    (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+OPTIONAL MATCH (samp)--&gt;(:participant)&lt;--(diag:diagnosis)
+WITH inputs, na, samp, data,
+	COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+WHERE
+    (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnoses, primary_diagnosis)) &gt; 0)
+RETURN 
+	data.sample_id AS `Sample ID`,
+	data.participant_id AS `Participant ID`,
+	data.study_name AS `Study Name`,
+	data.accession AS `Accession`,
+	data.tumor AS `Tumor`,
+	data.analyte_type AS `Analyte Type`
+ORDER BY `Sample ID`
+LIMIT 100</t>
+  </si>
+  <si>
+    <t>WITH {
+    phs_accession: "phs002250",
+    subject_ids: [],
+    experimental_strategies: [],
+    genders: ["Female"],
+    sample_tumor_statuses: ["Normal"],
+    file_types: [],
+    library_strategies: ["Not specified in data"],
+    library_sources: [],
+    library_selections: [],
+    library_layouts: [],
+    platforms: [],
+    instrument_models: [],
+    reference_genome_assemblies: [],
+    primary_diagnoses: [],
+    num_study_samples_min: 0,
+    num_study_samples_max: 0,
+    num_study_participants_max: 0,
+    num_study_participants_min: 0
+} AS inputs, "Not specified in data" AS na
+MATCH (s:study {phs_accession: inputs.phs_accession})
+OPTIONAL MATCH (s)&lt;--(p:participant)
+WITH inputs, na, s, count(distinct p) AS num_p
+WHERE
+    (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+    (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH inputs, na, s, count(distinct samp) AS num_samp
+WHERE
+    (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+    (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+MATCH (s)&lt;--(p:participant)
+WITH inputs, na, p, {
+	participant_id: coalesce(p.participant_id, ""),
+	study_name: coalesce(s.study_name, ""),
+	accession: coalesce(s.phs_accession, ""),
+	gender: coalesce(p.gender, "")
+} AS data
+WHERE 
+    (size(inputs.subject_ids) = 0 OR p.participant_id IN inputs.subject_ids) AND
+    (size(inputs.genders) = 0 OR p.gender IN inputs.genders)
 OPTIONAL MATCH (p)&lt;--(samp:sample)
-MATCH (samp)&lt;--(f:file)
-Match (f)&lt;--(g:genomic_info)
-WHERE s.study_name in ["CIDR: Discovery, Biology, and Risk of Inherited Variants in Glioma sample"] and 
-g.library_strategy in ['Not specified in data']and p.gender in['Female']and samp.sample_tumor_status in["Normal"]
-WITH p, s, collect(distinct samp.sample_id) as samp
+WITH inputs, na, p, apoc.map.merge(data, {
+		samples: coalesce(apoc.text.join(apoc.coll.sort(collect(distinct samp.sample_id)), ", "), "")
+	}) AS data,
+	COLLECT(DISTINCT samp.sample_tumor_status) AS sample_tumor_statuses
+WHERE
+    (size(inputs.sample_tumor_statuses) = 0 OR size(apoc.coll.intersection(inputs.sample_tumor_statuses, sample_tumor_statuses)) &gt; 0)
+OPTIONAL MATCH (p)&lt;--(:sample)&lt;--(f:file)
+WITH inputs, na, p, data,
+	COLLECT(DISTINCT f.file_type) AS file_types, 
+	apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+WHERE
+    (size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+    (size(inputs.file_types) = 0 OR size(apoc.coll.intersection(inputs.file_types, file_types)) &gt; 0)
+OPTIONAL MATCH (p)&lt;--(:sample)&lt;--(:file)&lt;--(g:genomic_info)
+WITH inputs, na, p, data,
+	COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+	COLLECT(DISTINCT g.library_source) AS library_source,
+	COLLECT(DISTINCT g.library_selection) AS library_selection,
+	COLLECT(DISTINCT g.library_layout) AS library_layout,
+	COLLECT(DISTINCT g.platform) AS platform,
+	COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+	COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+WHERE
+    (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+    (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND 
+    (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+    (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+    (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+    (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+    (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+WITH inputs, na, p, data,
+	COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+WHERE
+    (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnoses, primary_diagnosis)) &gt; 0)
+RETURN 
+	data.participant_id AS `Participant ID`,
+	data.study_name AS `Study Name`,
+	data.accession AS `Accession`,
+	data.gender AS `Gender`,
+	data.samples AS `Samples`
+ORDER BY `Participant ID`
+LIMIT 100</t>
+  </si>
+  <si>
+    <t>WITH {
+    phs_accession: "phs002250",
+    subject_ids: [],
+    experimental_strategies: [],
+    gender: ["Female"],
+    sample_tumor_statuses: ["Normal"],
+    file_types: [],
+    library_strategies: ["Not specified in data"],
+    library_sources: [],
+    library_selections: [],
+    library_layouts: [],
+    platforms: [],
+    instrument_models: [],
+    reference_genome_assemblies: [],
+    primary_diagnoses: [],
+    num_study_samples_min: 0,
+    num_study_samples_max: 0,
+    num_study_participants_max: 0,
+    num_study_participants_min: 0
+} AS inputs, "Not specified in data" AS na
+CALL{
+    WITH inputs, na
+    MATCH (s:study {phs_accession: inputs.phs_accession})
+    OPTIONAL MATCH (s)&lt;--(p:participant)
+    WITH inputs, na, s, count(distinct p) AS num_p
+    WHERE
+        (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+        (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+    OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+    WITH inputs, na, s, count(distinct samp) AS num_samp
+    WHERE
+        (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+        (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+    MATCH (s)&lt;--(p:participant)
+    WITH inputs, na, p
+    WHERE 
+        (size(inputs.subject_ids) = 0 OR p.participant_id IN inputs.subject_ids) AND
+        (size(inputs.gender) = 0 OR p.gender IN inputs.gender)
+    OPTIONAL MATCH (p)&lt;--(samp:sample)
+    WITH inputs, na, p,
+        COLLECT(DISTINCT samp.sample_tumor_status) AS sample_tumor_statuses
+    WHERE
+        (size(inputs.sample_tumor_statuses) = 0 OR size(apoc.coll.intersection(inputs.sample_tumor_statuses, sample_tumor_statuses)) &gt; 0)
+    OPTIONAL MATCH (p)&lt;--(:sample)&lt;--(f:file)
+    WITH inputs, na, p,
+        COLLECT(DISTINCT f.file_type) AS file_types, 
+        apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+    WHERE
+        (size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+        (size(inputs.file_types) = 0 OR size(apoc.coll.intersection(inputs.file_types, file_types)) &gt; 0)
+    OPTIONAL MATCH (p)&lt;--(:sample)&lt;--(:file)&lt;--(g:genomic_info)
+    WITH inputs, na, p,
+        COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+        COLLECT(DISTINCT g.library_source) AS library_source,
+        COLLECT(DISTINCT g.library_selection) AS library_selection,
+        COLLECT(DISTINCT g.library_layout) AS library_layout,
+        COLLECT(DISTINCT g.platform) AS platform,
+        COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+        COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+    WHERE
+        (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+        (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND 
+        (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+        (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+        (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+        (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+        (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+    OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+    WITH inputs, na, p,
+        COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+    WHERE
+        (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnoses, primary_diagnosis)) &gt; 0)
+    RETURN 
+        count(distinct p) AS num_participants
+    }
+WITH inputs, na, num_participants
+CALL {
+    WITH inputs, na
+    MATCH (s:study {phs_accession: inputs.phs_accession})
+    OPTIONAL MATCH (s)&lt;--(p:participant)
+    WITH inputs, na, s, count(distinct p) AS num_p
+    WHERE
+        (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+        (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+    OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+    WITH inputs, na, s, count(distinct samp) AS num_samp
+    WHERE
+        (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+        (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+    MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+    WITH inputs, na, samp
+    WHERE
+        (size(inputs.sample_tumor_statuses) = 0 OR samp.sample_tumor_status IN inputs.sample_tumor_statuses)
+    OPTIONAL MATCH (samp)--&gt;(p:participant)
+    WITH inputs, na, samp, 
+        COLLECT(DISTINCT p.participant_id) AS participant_id,
+        COLLECT(DISTINCT p.gender) AS gender
+    WHERE 
+        (size(inputs.subject_ids) = 0 OR size(apoc.coll.intersection(inputs.participant_id, participant_id)) &gt; 0) AND
+        (size(inputs.genders) = 0 OR size(apoc.coll.intersection(inputs.gender, gender)) &gt; 0)
+    OPTIONAL MATCH (samp)&lt;--(f:file)
+    WITH inputs, na, samp,
+        COLLECT(DISTINCT f.file_type) AS file_types, 
+        apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+    WHERE
+        (size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+        (size(inputs.file_types) = 0 OR size(apoc.coll.intersection(inputs.file_types, file_types)) &gt; 0)
+    OPTIONAL MATCH (samp)&lt;--(:file)&lt;--(g:genomic_info)
+    WITH inputs, na, samp,
+        COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+        COLLECT(DISTINCT g.library_source) AS library_source,
+        COLLECT(DISTINCT g.library_selection) AS library_selection,
+        COLLECT(DISTINCT g.library_layout) AS library_layout,
+        COLLECT(DISTINCT g.platform) AS platform,
+        COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+        COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+    WHERE
+        (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+        (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND 
+        (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+        (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+        (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+        (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+        (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+    OPTIONAL MATCH (samp)--&gt;(:participant)&lt;--(diag:diagnosis)
+    WITH inputs, na, samp,
+        COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+    WHERE
+        (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnoses, primary_diagnosis)) &gt; 0)
+    RETURN 
+        count(distinct samp) AS num_samples
+}
+WITH inputs, na, num_participants, num_samples
+CALL {
+    WITH inputs, na
+    MATCH (s:study {phs_accession: inputs.phs_accession})
+    OPTIONAL MATCH (s)&lt;--(p:participant)
+    WITH inputs, na, s, count(distinct p) AS num_p
+    WHERE
+        (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+        (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+    OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+    WITH inputs, na, s, count(distinct samp) AS num_samp
+    WHERE
+        (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+        (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+    MATCH (s)&lt;--(f:file)
+    WITH inputs, na, f,
+        apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+    WHERE 
+        (size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+        (size(inputs.file_types) = 0 OR f.file_type IN inputs.file_types)
+    OPTIONAL MATCH (f)--&gt;(samp)
+    WITH inputs, na, f,
+        COLLECT(DISTINCT samp.sample_tumor_status) AS sample_tumor_status
+    WHERE
+        (size(inputs.sample_tumor_statuses) = 0 OR size(apoc.coll.intersection(inputs.sample_tumor_statuses, sample_tumor_status)) &gt; 0)
+    OPTIONAL MATCH (f)--&gt;(:sample)--&gt;(p:participant)
+    WITH inputs, na, f, 
+        COLLECT(DISTINCT p.participant_id) AS participant_id,
+        COLLECT(DISTINCT p.gender) AS gender
+    WHERE 
+        (size(inputs.subject_ids) = 0 OR size(apoc.coll.intersection(inputs.participant_id, participant_id)) &gt; 0) AND
+        (size(inputs.genders) = 0 OR size(apoc.coll.intersection(inputs.gender, gender)) &gt; 0)
+    OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+    WITH inputs, na, f,
+        COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+        COLLECT(DISTINCT g.library_source) AS library_source,
+        COLLECT(DISTINCT g.library_selection) AS library_selection,
+        COLLECT(DISTINCT g.library_layout) AS library_layout,
+        COLLECT(DISTINCT g.platform) AS platform,
+        COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+        COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+    WHERE
+        (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+        (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND 
+        (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+        (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+        (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+        (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+        (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+    OPTIONAL MATCH (f)--&gt;(:sample)--&gt;(:participant)&lt;--(diag:diagnosis)
+    WITH inputs, na, f,
+        COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+    WHERE
+        (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnoses, primary_diagnosis)) &gt; 0)
+    RETURN 
+        count(distinct f) AS num_files
+}
 RETURN
- coalesce(p.participant_id,'') as `Participant ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(p.gender,'') as `Gender`,
- coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER By p.participant_id LIMIT 100</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-Match (f)&lt;--(g:genomic_info)
-WITH DISTINCT samp,diag,s,p,g,f
-WHERE s.study_name in ["CIDR: Discovery, Biology, and Risk of Inherited Variants in Glioma sample"] and g.library_strategy in ['Not specified in data'] and p.gender in['Female']and samp.sample_tumor_status in["Normal"]
-RETURN
-    count(distinct s) AS Studies,
-    count(distinct p) AS Participants,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS Files</t>
-  </si>
-  <si>
-    <t>TC02_CDS_study-CIDR_LibraryStrategy-NotSpecifiedindata_Gender-Female_SampleTumor-Normal_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC02_CDS_study-CIDR_LibraryStrategy-NotSpecifiedindata_Gender-Female_SampleTumor-Normal_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-Match (f)&lt;--(g:genomic_info)
-WITH DISTINCT samp,diag,s,p,g,f
-WHERE s.study_name in ["CIDR: Discovery, Biology, and Risk of Inherited Variants in Glioma sample"] and g.library_strategy in ['Not specified in data'] and p.gender in['Female'] and samp.sample_tumor_status in["Normal"]
-RETURN
-    count(distinct s) AS Studies,
-    count(distinct p) AS Participants,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS Files</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
- MATCH  (samp)&lt;--(f:file)
-Match (f)&lt;--(g:genomic_info)
-WHERE s.study_name in ["CIDR: Discovery, Biology, and Risk of Inherited Variants in Glioma sample"] and g.library_strategy in ['Not specified in data']and p.gender in['Female'] and samp.sample_tumor_status in["Normal"]
-WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
-RETURN
- coalesce(samp.sample_id, '') as `Sample ID`,
- coalesce(p.participant_id,'') as `Participant ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(samp.sample_tumor_status,'') as `Tumor`,
-coalesce(samp.sample_type,'') as `Analyte Type`
-ORDER By samp.sample_id LIMIT 100</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
-MATCH (samp)&lt;--(f:file)
-Match (f)&lt;--(g:genomic_info)
-WHERE s.study_name in ["CIDR: Discovery, Biology, and Risk of Inherited Variants in Glioma sample"] and g.library_strategy in ['Not specified in data']and p.gender in['Female'] and samp.sample_tumor_status in["Normal"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT p,s,samp,f,diag
+    1 AS Studies,
+    num_participants AS Participants,
+    num_samples AS Samples,
+    num_files AS `Files`</t>
+  </si>
+  <si>
+    <t>WITH {
+    phs_accession: "phs002250",
+    subject_ids: [],
+    experimental_strategies: ["WGS"],
+    genders: ["Female"],
+    sample_tumor_statuses: ["Normal"],
+    file_types: [],
+    library_strategies: ["Not specified in data"],
+    library_sources: [],
+    library_selections: [],
+    library_layouts: [],
+    platforms: [],
+    instrument_models: [],
+    reference_genome_assemblies: [],
+    primary_diagnoses: [],
+    num_study_samples_min: 0,
+    num_study_samples_max: 0,
+    num_study_participants_max: 0,
+    num_study_participants_min: 0
+} AS inputs, "Not specified in data" AS na
+MATCH (s:study {phs_accession: inputs.phs_accession})
+OPTIONAL MATCH (s)&lt;--(p:participant)
+WITH inputs, na, s, count(distinct p) AS num_p
+WHERE
+    (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+    (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH inputs, na, s, count(distinct samp) AS num_samp
+WHERE
+    (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+    (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+MATCH (s)&lt;--(f:file)
+WITH inputs, na, f, {
+        file_name: coalesce(f.file_name, ""),
+        file_type: coalesce(f.file_type, ""),
+        study_name: coalesce(s.study_name, ""),
+        accession: coalesce(s.phs_accession, "")
+    } AS data,
+    apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+WHERE 
+    (size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+    (size(inputs.file_types) = 0 OR f.file_type IN inputs.file_types)
+OPTIONAL MATCH (f)--&gt;(samp)
+WITH inputs, na, f, apoc.map.merge(data, {
+        sample_id: coalesce(apoc.text.join(apoc.coll.sort(collect(distinct samp.sample_id)), ", "), "")
+    }) AS data,
+    COLLECT(DISTINCT samp.sample_tumor_status) AS sample_tumor_status
+WHERE
+    (size(inputs.sample_tumor_statuses) = 0 OR size(apoc.coll.intersection(inputs.sample_tumor_statuses, sample_tumor_status)) &gt; 0)
+OPTIONAL MATCH (f)--&gt;(:sample)--&gt;(p:participant)
+WITH inputs, na, f, 
+    apoc.map.merge(data, {
+        participant_id: coalesce(apoc.text.join(collect(distinct p.participant_id), ", "), "")
+    }) AS data,
+    COLLECT(DISTINCT p.participant_id) AS participant_id,
+    COLLECT(DISTINCT p.gender) AS gender
+WHERE 
+    (size(inputs.subject_ids) = 0 OR size(apoc.coll.intersection(inputs.subject_ids, participant_id)) &gt; 0) AND
+    (size(inputs.genders) = 0 OR size(apoc.coll.intersection(inputs.genders, gender)) &gt; 0)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+WITH inputs, na, f, data,
+    COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+    COLLECT(DISTINCT g.library_source) AS library_source,
+    COLLECT(DISTINCT g.library_selection) AS library_selection,
+    COLLECT(DISTINCT g.library_layout) AS library_layout,
+    COLLECT(DISTINCT g.platform) AS platform,
+    COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+    COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+WHERE
+    (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+    (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND 
+    (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+    (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+    (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+    (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+    (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+OPTIONAL MATCH (f)--&gt;(:sample)--&gt;(:participant)&lt;--(diag:diagnosis)
+WITH inputs, na, f, data,
+    COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+WHERE
+    (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnoses, primary_diagnosis)) &gt; 0)
 RETURN 
-    coalesce(f.file_name, '') as `File Name`,
-    coalesce(s.study_name, '') as `Study Name`,
-    coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(p.participant_id,'') as `Subject ID`,
-    coalesce(samp.sample_id, '') as `Sample ID`,
-    coalesce(f.file_type, '') as `File Type`
-   ORDER By f.file_name LIMIT 100</t>
+    data.file_name AS `File Name`,
+    data.study_name AS `Study Name`,
+    data.accession AS `Accession`,
+    data.participant_id AS `Participant Id`,
+    data.sample_id AS `Sample Id`,
+    data.file_type AS `File Type`
+ORDER BY `File Name`
+LIMIT 100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +561,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -194,12 +590,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -520,22 +920,23 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.1796875" customWidth="1"/>
-    <col min="5" max="5" width="63.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" customWidth="1"/>
+    <col min="5" max="5" width="63.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -548,58 +949,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="248" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="232.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="279" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
       <c r="C5" s="1"/>
     </row>
   </sheetData>

</xml_diff>